<commit_message>
Report des propriétés / méthodes (membres) dans les classes à partir du diagramme.
</commit_message>
<xml_diff>
--- a/asset/diagram.xlsx
+++ b/asset/diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/TP_Villes_du_Monde/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D253B89-48E2-BF41-8DD1-8414B07B4C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDA8604-0E6D-754D-B10C-2A448BE6A8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{8735055C-E134-3E4D-82DA-80B73531BE17}"/>
+    <workbookView xWindow="38000" yWindow="2140" windowWidth="28800" windowHeight="16380" xr2:uid="{8735055C-E134-3E4D-82DA-80B73531BE17}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagram" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="101">
   <si>
     <t>dataSource</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>Surcharge la méthode et définit une classe CSS en plus de la méthode de base.</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -659,18 +662,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -680,7 +671,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -771,6 +761,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -780,9 +785,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1374,8 +1377,8 @@
   </sheetPr>
   <dimension ref="A2:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="59" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="J18" zoomScale="166" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1398,21 +1401,21 @@
   <sheetData>
     <row r="2" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
-      <c r="G3" s="16" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="56"/>
+      <c r="G3" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
-      <c r="K3" s="16" t="s">
+      <c r="H3" s="55"/>
+      <c r="I3" s="56"/>
+      <c r="K3" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="18"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="56"/>
     </row>
     <row r="4" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="str">
@@ -1453,107 +1456,107 @@
       </c>
     </row>
     <row r="5" spans="2:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="38" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="14"/>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="24" t="s">
         <v>26</v>
       </c>
       <c r="I5" s="13"/>
-      <c r="K5" s="38" t="s">
+      <c r="K5" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="43" t="s">
+      <c r="L5" s="38" t="s">
         <v>8</v>
       </c>
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="2:15" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="G6" s="30" t="s">
+      <c r="D6" s="19"/>
+      <c r="G6" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="38" t="s">
+      <c r="H6" s="33" t="s">
         <v>28</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="48" t="s">
+      <c r="L6" s="43" t="s">
         <v>20</v>
       </c>
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="2:15" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="G7" s="42" t="s">
+      <c r="D7" s="20"/>
+      <c r="G7" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="51" t="s">
+      <c r="H7" s="46" t="s">
         <v>27</v>
       </c>
       <c r="I7" s="5"/>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="48"/>
+      <c r="L7" s="43"/>
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="2:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="23"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="43" t="s">
+      <c r="L8" s="38" t="s">
         <v>21</v>
       </c>
       <c r="M8" s="14"/>
     </row>
     <row r="9" spans="2:15" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="41" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
-      <c r="K9" s="32" t="s">
+      <c r="K9" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="46" t="s">
+      <c r="L9" s="41" t="s">
         <v>22</v>
       </c>
       <c r="M9" s="3"/>
@@ -1600,9 +1603,9 @@
       <c r="F14" s="10"/>
       <c r="G14" s="9"/>
       <c r="J14" s="9"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="57"/>
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
     </row>
@@ -1677,16 +1680,16 @@
       <c r="O19" s="9"/>
     </row>
     <row r="20" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="E20" s="16" t="s">
+      <c r="B20" s="55"/>
+      <c r="C20" s="56"/>
+      <c r="E20" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="56"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -1695,7 +1698,7 @@
       <c r="O20" s="9"/>
     </row>
     <row r="21" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="str">
+      <c r="A21" s="21" t="str">
         <f>Param!A1</f>
         <v>Properties / Methods</v>
       </c>
@@ -1721,27 +1724,31 @@
       </c>
       <c r="J21" s="9"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="16" t="s">
+      <c r="O21" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="18"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="56"/>
     </row>
     <row r="22" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="E22" s="29" t="s">
+      <c r="C22" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="F22" s="43" t="s">
+      <c r="F22" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="13"/>
+      <c r="G22" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="I22" s="58" t="s">
         <v>29</v>
       </c>
@@ -1762,319 +1769,389 @@
       </c>
     </row>
     <row r="23" spans="1:17" ht="120" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="E23" s="38" t="s">
+      <c r="C23" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="F23" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="I23" s="51" t="str">
+      <c r="G23" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I23" s="46" t="str">
         <f>Param!A1</f>
         <v>Properties / Methods</v>
       </c>
-      <c r="J23" s="61" t="str">
+      <c r="J23" s="53" t="str">
         <f>Param!A2</f>
         <v>Description</v>
       </c>
-      <c r="K23" s="51" t="str">
+      <c r="K23" s="46" t="str">
         <f>Param!A3</f>
         <v>Checked</v>
       </c>
       <c r="N23" s="9"/>
-      <c r="O23" s="51" t="s">
+      <c r="O23" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="P23" s="57" t="s">
+      <c r="P23" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="Q23" s="3"/>
-    </row>
-    <row r="24" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="35" t="s">
+      <c r="Q23" s="61" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="E24" s="38" t="s">
+      <c r="C24" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="F24" s="48" t="s">
+      <c r="F24" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="I24" s="29" t="s">
+      <c r="G24" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I24" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="J24" s="52" t="s">
+      <c r="J24" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="13"/>
+      <c r="K24" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
-      <c r="P24" s="20"/>
+      <c r="P24" s="16"/>
       <c r="Q24" s="9"/>
     </row>
-    <row r="25" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="34" t="s">
+    <row r="25" spans="1:17" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="E25" s="30" t="s">
+      <c r="C25" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="F25" s="44" t="s">
+      <c r="F25" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="G25" s="8"/>
-      <c r="I25" s="38" t="s">
+      <c r="G25" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="I25" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="J25" s="52" t="s">
+      <c r="J25" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="K25" s="4"/>
+      <c r="K25" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
-      <c r="P25" s="20"/>
+      <c r="P25" s="16"/>
       <c r="Q25" s="9"/>
     </row>
-    <row r="26" spans="1:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="36" t="s">
+    <row r="26" spans="1:17" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="E26" s="39" t="s">
+      <c r="C26" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="F26" s="49" t="s">
+      <c r="F26" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="G26" s="28"/>
-      <c r="I26" s="38" t="s">
+      <c r="G26" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="I26" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="52" t="s">
+      <c r="J26" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="K26" s="4"/>
+      <c r="K26" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="O26" s="9"/>
-      <c r="P26" s="20"/>
+      <c r="P26" s="16"/>
       <c r="Q26" s="9"/>
     </row>
-    <row r="27" spans="1:17" ht="102" x14ac:dyDescent="0.2">
-      <c r="A27" s="36" t="s">
+    <row r="27" spans="1:17" ht="103" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="E27" s="40" t="s">
+      <c r="C27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="47" t="s">
+      <c r="F27" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="G27" s="4"/>
-      <c r="I27" s="40" t="s">
+      <c r="G27" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I27" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="52" t="s">
+      <c r="J27" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="K27" s="4"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="22"/>
+      <c r="K27" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="O27" s="17"/>
+      <c r="P27" s="18"/>
       <c r="Q27" s="9"/>
     </row>
-    <row r="28" spans="1:17" ht="153" x14ac:dyDescent="0.2">
-      <c r="A28" s="36" t="s">
+    <row r="28" spans="1:17" ht="154" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="E28" s="41" t="s">
+      <c r="C28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="50" t="s">
+      <c r="F28" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="G28" s="8"/>
-      <c r="I28" s="53" t="s">
+      <c r="G28" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="I28" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="J28" s="54" t="s">
+      <c r="J28" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="K28" s="25"/>
+      <c r="K28" s="13" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="29" spans="1:17" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="E29" s="40" t="s">
+      <c r="C29" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="47" t="s">
+      <c r="F29" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="G29" s="4"/>
-      <c r="I29" s="40" t="s">
+      <c r="G29" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I29" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="J29" s="55" t="s">
+      <c r="J29" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="K29" s="4"/>
-    </row>
-    <row r="30" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="E30" s="40" t="s">
+      <c r="K29" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="F30" s="47" t="s">
+      <c r="F30" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="G30" s="4"/>
-      <c r="I30" s="40" t="s">
+      <c r="G30" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I30" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="J30" s="55" t="s">
+      <c r="J30" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="K30" s="4"/>
-    </row>
-    <row r="31" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="E31" s="40" t="s">
+      <c r="K30" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="F31" s="47" t="s">
+      <c r="F31" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="G31" s="4"/>
-      <c r="I31" s="40" t="s">
+      <c r="G31" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I31" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="J31" s="55" t="s">
+      <c r="J31" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="K31" s="4"/>
-    </row>
-    <row r="32" spans="1:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="E32" s="40" t="s">
+      <c r="K31" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="47" t="s">
+      <c r="F32" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="G32" s="4"/>
-      <c r="I32" s="40" t="s">
+      <c r="G32" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I32" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="J32" s="55" t="s">
+      <c r="J32" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="K32" s="4"/>
-    </row>
-    <row r="33" spans="5:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="E33" s="40" t="s">
+      <c r="K32" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="5:11" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="F33" s="47" t="s">
+      <c r="F33" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="G33" s="4"/>
-      <c r="I33" s="40" t="s">
+      <c r="G33" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I33" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="J33" s="55" t="s">
+      <c r="J33" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K33" s="4"/>
+      <c r="K33" s="13" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="34" spans="5:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E34" s="32" t="s">
+      <c r="E34" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="F34" s="46" t="s">
+      <c r="F34" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="G34" s="5"/>
-      <c r="I34" s="40" t="s">
+      <c r="G34" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I34" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="J34" s="55" t="s">
+      <c r="J34" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="K34" s="4"/>
-    </row>
-    <row r="35" spans="5:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="I35" s="40" t="s">
+      <c r="K34" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="5:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="J35" s="55" t="s">
+      <c r="J35" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="K35" s="4"/>
-    </row>
-    <row r="36" spans="5:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="I36" s="40" t="s">
+      <c r="K35" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="5:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="J36" s="55" t="s">
+      <c r="J36" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="K36" s="4"/>
-    </row>
-    <row r="37" spans="5:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="I37" s="40" t="s">
+      <c r="K36" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="5:11" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I37" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="J37" s="55" t="s">
+      <c r="J37" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="K37" s="4"/>
+      <c r="K37" s="13" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="38" spans="5:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I38" s="32" t="s">
+      <c r="I38" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="J38" s="56" t="s">
+      <c r="J38" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="K38" s="5"/>
+      <c r="K38" s="13" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="E20:G20"/>
     <mergeCell ref="O21:Q21"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="K14:M14"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="E20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="29" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>